<commit_message>
fix a logical import
</commit_message>
<xml_diff>
--- a/preguntas_razonamiento.xlsx
+++ b/preguntas_razonamiento.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhernandezm/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhernandezm/sites/compass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32BF2FE-5A2F-B845-9B70-D09995B1E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB3FC7-353D-1E4E-B9AC-311A10630943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="46080" windowHeight="25420" xr2:uid="{33624FCC-EBD3-6D43-BA9E-DBC944FE1FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>question_image</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>correct_answer</t>
@@ -357,256 +354,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6616700" y="203200"/>
-          <a:ext cx="209903" cy="215900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1312670</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagen 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A74687C-AF8F-C50B-3C6A-CF2740C9B073}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="406400"/>
-          <a:ext cx="1312670" cy="215900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5347</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Imagen 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F17CC8AF-0172-B8C7-0337-EE9A0E8E1AA3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1638300" y="406400"/>
-          <a:ext cx="203200" cy="208547"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>200416</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Imagen 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71974A5-8E7E-D272-FC09-C07D1ACFA101}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3136900" y="406400"/>
-          <a:ext cx="203200" cy="200416"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180269</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagen 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{207E9252-6F55-6A75-F128-9A25E5FFC578}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4876800" y="406400"/>
-          <a:ext cx="180269" cy="177800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209903</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Imagen 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A60FEAFD-C48B-4AC1-0D17-2B8587A71FCC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6616700" y="406400"/>
           <a:ext cx="209903" cy="215900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -936,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CC124D-3143-164D-8EE4-0EC578015AF3}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -976,11 +723,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fix a importacion de reazonamiento
</commit_message>
<xml_diff>
--- a/preguntas_razonamiento.xlsx
+++ b/preguntas_razonamiento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhernandezm/sites/compass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB3FC7-353D-1E4E-B9AC-311A10630943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C839559-C281-7245-B14F-9859D97C4B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="46080" windowHeight="25420" xr2:uid="{33624FCC-EBD3-6D43-BA9E-DBC944FE1FE2}"/>
+    <workbookView xWindow="860" yWindow="2600" windowWidth="38400" windowHeight="21100" xr2:uid="{33624FCC-EBD3-6D43-BA9E-DBC944FE1FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>question_image</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>correct_answer</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -355,6 +358,256 @@
         <a:xfrm>
           <a:off x="6616700" y="203200"/>
           <a:ext cx="209903" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>199572</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>172358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>979715</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>13487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D18D56A-FBE3-B2B8-E063-B79110E520A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="199572" y="371929"/>
+          <a:ext cx="780143" cy="240272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9072</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>172358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>217911</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F145A882-B335-9E0A-41FC-FDB54A3E96F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6631215" y="371929"/>
+          <a:ext cx="208839" cy="290286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>13929</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>18143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6508A1AA-DE3B-7429-84EA-F8079A92E6CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4894358" y="376786"/>
+          <a:ext cx="205485" cy="240071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9716</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>182074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>233739</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC5D572D-0620-FAE5-9BE5-D92C2176BFAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3148430" y="381645"/>
+          <a:ext cx="224023" cy="262427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1638358</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>186929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>201909</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9072</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagen 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{778C91C3-78C7-AF09-C0B8-5B9DBF0D8095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638358" y="386500"/>
+          <a:ext cx="205480" cy="221286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -683,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CC124D-3143-164D-8EE4-0EC578015AF3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,6 +976,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>